<commit_message>
Termine todo, gracias capo
</commit_message>
<xml_diff>
--- a/Practicos/labfinal/medidas.xlsx
+++ b/Practicos/labfinal/medidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://finguy-my.sharepoint.com/personal/federico_gil_fing_edu_uy/Documents/Escritorio/Facultad/Semestre 11/GPGPU/Practico 1/cositas/GPGPU/Practicos/labfinal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="8_{E4A5B43A-06FE-4F9F-B088-4855B00F055B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{814FE6FE-7EEB-44E2-873F-98CE2B71C80D}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="8_{E4A5B43A-06FE-4F9F-B088-4855B00F055B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{194F2C90-EA00-4D3A-AF39-7F7D5C34AB3A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8BB1CD6E-8E1A-4958-B8CA-22BA6FE3242E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
   <si>
     <t>1.pgm</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Network</t>
+  </si>
+  <si>
+    <t>Countsort</t>
+  </si>
+  <si>
+    <t>Shell</t>
   </si>
 </sst>
 </file>
@@ -281,10 +287,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,58 +631,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844EDFC7-8DC0-4A83-AF74-6C1538609742}">
-  <dimension ref="B1:R17"/>
+  <dimension ref="B1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H23" sqref="F19:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="16" width="10.42578125" customWidth="1"/>
-    <col min="17" max="18" width="11.140625" customWidth="1"/>
+    <col min="3" max="20" width="10.42578125" customWidth="1"/>
+    <col min="21" max="22" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="14"/>
+      <c r="H2" s="13"/>
       <c r="I2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="14"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="14"/>
+      <c r="N2" s="13"/>
       <c r="O2" s="12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="P2" s="13"/>
       <c r="Q2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="13"/>
+      <c r="S2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="14"/>
+      <c r="U2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="13"/>
+      <c r="V2" s="14"/>
     </row>
-    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -719,17 +733,29 @@
       <c r="O3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -770,19 +796,31 @@
         <v>3.0360000000000002E-2</v>
       </c>
       <c r="O4" s="7">
+        <v>0.4768</v>
+      </c>
+      <c r="P4" s="9">
+        <v>2.0929999999999998E-3</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>13.911899999999999</v>
+      </c>
+      <c r="R4" s="9">
+        <v>1.38442</v>
+      </c>
+      <c r="S4" s="7">
         <v>5.6640000000000003E-2</v>
       </c>
-      <c r="P4" s="8">
+      <c r="T4" s="8">
         <v>5.9389999999999996E-4</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="U4" s="10">
         <v>4.0627200000000002E-2</v>
       </c>
-      <c r="R4" s="8">
+      <c r="V4" s="8">
         <v>8.1400000000000005E-4</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>5</v>
       </c>
@@ -823,19 +861,31 @@
         <v>0.11409999999999999</v>
       </c>
       <c r="O5" s="7">
+        <v>2.5136799999999999</v>
+      </c>
+      <c r="P5" s="9">
+        <v>7.7200000000000003E-3</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>18.22</v>
+      </c>
+      <c r="R5" s="9">
+        <v>1.4342999999999999</v>
+      </c>
+      <c r="S5" s="7">
         <v>0.55159999999999998</v>
       </c>
-      <c r="P5" s="8">
+      <c r="T5" s="8">
         <v>1.196E-3</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="U5" s="10">
         <v>9.8549999999999999E-2</v>
       </c>
-      <c r="R5" s="8">
+      <c r="V5" s="8">
         <v>8.3900000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>7</v>
       </c>
@@ -876,19 +926,31 @@
         <v>2.1215999999999999E-2</v>
       </c>
       <c r="O6" s="7">
+        <v>8.3865599999999993</v>
+      </c>
+      <c r="P6" s="9">
+        <v>1.512E-2</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>19.829999999999998</v>
+      </c>
+      <c r="R6" s="9">
+        <v>1.2410000000000001</v>
+      </c>
+      <c r="S6" s="7">
         <v>2.0009999999999999</v>
       </c>
-      <c r="P6" s="8">
+      <c r="T6" s="8">
         <v>3.90625E-3</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="U6" s="10">
         <v>0.76276999999999995</v>
       </c>
-      <c r="R6" s="8">
+      <c r="V6" s="8">
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>9</v>
       </c>
@@ -929,15 +991,27 @@
         <v>6.3709000000000002E-2</v>
       </c>
       <c r="O7" s="7">
+        <v>21.6494</v>
+      </c>
+      <c r="P7" s="9">
+        <v>0.82120000000000004</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>18.2622</v>
+      </c>
+      <c r="R7" s="9">
+        <v>1.2542</v>
+      </c>
+      <c r="S7" s="7">
         <v>5.6428099999999999</v>
       </c>
-      <c r="P7" s="8">
+      <c r="T7" s="8">
         <v>1.9530000000000001E-3</v>
       </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="8"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="8"/>
     </row>
-    <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>11</v>
       </c>
@@ -978,53 +1052,73 @@
         <v>0.63739999999999997</v>
       </c>
       <c r="O8" s="5">
+        <v>30.492799999999999</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.9728</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>25.110199999999999</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1.2696000000000001</v>
+      </c>
+      <c r="S8" s="5">
         <v>12.561999999999999</v>
       </c>
-      <c r="P8" s="6">
+      <c r="T8" s="6">
         <v>1.9529999999999999E-2</v>
       </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="6"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="6"/>
     </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="13"/>
       <c r="I11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="13"/>
       <c r="K11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="14"/>
+      <c r="L11" s="13"/>
       <c r="M11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="14"/>
+      <c r="N11" s="13"/>
       <c r="O11" s="12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="R11" s="13"/>
+      <c r="S11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" s="14"/>
+      <c r="U11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R11" s="13"/>
+      <c r="V11" s="14"/>
     </row>
-    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1067,17 +1161,29 @@
       <c r="O12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P12" s="6" t="s">
+      <c r="P12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="Q12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="R12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="V12" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -1118,19 +1224,31 @@
         <v>0.69740000000000002</v>
       </c>
       <c r="O13" s="7">
+        <v>15.3309</v>
+      </c>
+      <c r="P13" s="9">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>425.80399999999997</v>
+      </c>
+      <c r="R13" s="9">
+        <v>2.95275</v>
+      </c>
+      <c r="S13" s="7">
         <v>1.35</v>
       </c>
-      <c r="P13" s="8">
+      <c r="T13" s="8">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="U13" s="10">
         <v>1.3250299999999999</v>
       </c>
-      <c r="R13" s="8">
+      <c r="V13" s="8">
         <v>1.0357999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>5</v>
       </c>
@@ -1171,19 +1289,31 @@
         <v>5.8400000000000001E-2</v>
       </c>
       <c r="O14" s="7">
+        <v>67.694000000000003</v>
+      </c>
+      <c r="P14" s="9">
+        <v>1.94</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>623.42399999999998</v>
+      </c>
+      <c r="R14" s="9">
+        <v>2.4811000000000001</v>
+      </c>
+      <c r="S14" s="7">
         <v>14.425599999999999</v>
       </c>
-      <c r="P14" s="8">
+      <c r="T14" s="8">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="U14" s="10">
         <v>3.43858</v>
       </c>
-      <c r="R14" s="8">
+      <c r="V14" s="8">
         <v>1.3810000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>7</v>
       </c>
@@ -1224,19 +1354,31 @@
         <v>0</v>
       </c>
       <c r="O15" s="7">
+        <v>222.756</v>
+      </c>
+      <c r="P15" s="9">
+        <v>0.108253</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>681.93600000000004</v>
+      </c>
+      <c r="R15" s="9">
+        <v>1.0458000000000001</v>
+      </c>
+      <c r="S15" s="7">
         <v>52.407800000000002</v>
       </c>
-      <c r="P15" s="8">
+      <c r="T15" s="8">
         <v>1.5625E-2</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="U15" s="10">
         <v>26.022099999999998</v>
       </c>
-      <c r="R15" s="8">
+      <c r="V15" s="8">
         <v>1.3731599999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>9</v>
       </c>
@@ -1276,16 +1418,28 @@
       <c r="N16" s="9">
         <v>0.17677000000000001</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="7">
+        <v>602.70899999999995</v>
+      </c>
+      <c r="P16" s="9">
+        <v>12.0649</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>605.97500000000002</v>
+      </c>
+      <c r="R16" s="9">
+        <v>7.5124899999999997</v>
+      </c>
+      <c r="S16" s="10">
         <v>149.31299999999999</v>
       </c>
-      <c r="P16" s="8">
+      <c r="T16" s="8">
         <v>0.108253</v>
       </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="8"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="8"/>
     </row>
-    <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>11</v>
       </c>
@@ -1325,34 +1479,51 @@
       <c r="N17" s="4">
         <v>3.0413000000000001</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="5">
+        <v>934.52499999999998</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>823.43200000000002</v>
+      </c>
+      <c r="R17" s="4">
+        <v>8.45946</v>
+      </c>
+      <c r="S17" s="11">
         <v>328.07400000000001</v>
       </c>
-      <c r="P17" s="6">
+      <c r="T17" s="6">
         <v>0</v>
       </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="6"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
+  <mergeCells count="20">
     <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="S11:T11"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>